<commit_message>
Update formula when perform on the other sheet.
</commit_message>
<xml_diff>
--- a/Formula_Convert_Horizon2Vertical.xlsx
+++ b/Formula_Convert_Horizon2Vertical.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="0" windowWidth="27855" windowHeight="11820"/>
+    <workbookView xWindow="4725" yWindow="0" windowWidth="27855" windowHeight="11820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="22">
   <si>
     <t>a</t>
   </si>
@@ -617,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H13" workbookViewId="0">
-      <selection activeCell="AA15" sqref="AA15"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2203,4 +2204,541 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:K21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="31" t="str">
+        <f ca="1">IF(J3="","",SUBSTITUTE(J3,", ","",(LEN(J3)-LEN(SUBSTITUTE(J3,", ","")))/2))</f>
+        <v>X, Y</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5" t="str">
+        <f ca="1">IF(K3="","",SUBSTITUTE(K3,", ","",(LEN(K3)-LEN(SUBSTITUTE(K3,", ","")))/2))</f>
+        <v/>
+      </c>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="J3" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$17,B3+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$21,B3+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$25,B3+2))="n","Z, ","")</f>
+        <v xml:space="preserve">X, Y, </v>
+      </c>
+      <c r="K3" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$18,B3+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$22,B3+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$26,B3+2))="n","Z, ","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+      <c r="C4" s="31" t="str">
+        <f ca="1">IF(J4="","",SUBSTITUTE(J4,", ","",(LEN(J4)-LEN(SUBSTITUTE(J4,", ","")))/2))</f>
+        <v>Y</v>
+      </c>
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5" t="str">
+        <f t="shared" ref="E4:E20" ca="1" si="0">IF(K4="","",SUBSTITUTE(K4,", ","",(LEN(K4)-LEN(SUBSTITUTE(K4,", ","")))/2))</f>
+        <v>X, Y, Z</v>
+      </c>
+      <c r="F4" s="5">
+        <v>2</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="J4" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$17,B4+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$21,B4+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$25,B4+2))="n","Z, ","")</f>
+        <v xml:space="preserve">Y, </v>
+      </c>
+      <c r="K4" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$18,B4+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$22,B4+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$26,B4+2))="n","Z, ","")</f>
+        <v xml:space="preserve">X, Y, Z, </v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="31" t="str">
+        <f ca="1">IF(J5="","",SUBSTITUTE(J5,", ","",(LEN(J5)-LEN(SUBSTITUTE(J5,", ","")))/2))</f>
+        <v/>
+      </c>
+      <c r="D5" s="5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="F5" s="5">
+        <v>3</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="J5" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$17,B5+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$21,B5+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$25,B5+2))="n","Z, ","")</f>
+        <v/>
+      </c>
+      <c r="K5" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$18,B5+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$22,B5+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$26,B5+2))="n","Z, ","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="5">
+        <v>4</v>
+      </c>
+      <c r="C6" s="31" t="str">
+        <f ca="1">IF(J6="","",SUBSTITUTE(J6,", ","",(LEN(J6)-LEN(SUBSTITUTE(J6,", ","")))/2))</f>
+        <v>Z</v>
+      </c>
+      <c r="D6" s="5">
+        <v>4</v>
+      </c>
+      <c r="E6" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>X, Y, Z</v>
+      </c>
+      <c r="F6" s="5">
+        <v>4</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="J6" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$17,B6+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$21,B6+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$25,B6+2))="n","Z, ","")</f>
+        <v xml:space="preserve">Z, </v>
+      </c>
+      <c r="K6" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$18,B6+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$22,B6+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$26,B6+2))="n","Z, ","")</f>
+        <v xml:space="preserve">X, Y, Z, </v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="5">
+        <v>5</v>
+      </c>
+      <c r="C7" s="31" t="str">
+        <f ca="1">IF(J7="","",SUBSTITUTE(J7,", ","",(LEN(J7)-LEN(SUBSTITUTE(J7,", ","")))/2))</f>
+        <v>Z</v>
+      </c>
+      <c r="D7" s="5">
+        <v>5</v>
+      </c>
+      <c r="E7" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="F7" s="5">
+        <v>5</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="J7" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$17,B7+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$21,B7+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$25,B7+2))="n","Z, ","")</f>
+        <v xml:space="preserve">Z, </v>
+      </c>
+      <c r="K7" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$18,B7+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$22,B7+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$26,B7+2))="n","Z, ","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="5">
+        <v>6</v>
+      </c>
+      <c r="C8" s="31" t="str">
+        <f ca="1">IF(J8="","",SUBSTITUTE(J8,", ","",(LEN(J8)-LEN(SUBSTITUTE(J8,", ","")))/2))</f>
+        <v>X, Y, Z</v>
+      </c>
+      <c r="D8" s="5">
+        <v>6</v>
+      </c>
+      <c r="E8" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="F8" s="5">
+        <v>6</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="J8" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$17,B8+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$21,B8+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$25,B8+2))="n","Z, ","")</f>
+        <v xml:space="preserve">X, Y, Z, </v>
+      </c>
+      <c r="K8" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$18,B8+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$22,B8+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$26,B8+2))="n","Z, ","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="5">
+        <v>7</v>
+      </c>
+      <c r="C9" s="31" t="str">
+        <f ca="1">IF(J9="","",SUBSTITUTE(J9,", ","",(LEN(J9)-LEN(SUBSTITUTE(J9,", ","")))/2))</f>
+        <v>Z</v>
+      </c>
+      <c r="D9" s="5">
+        <v>7</v>
+      </c>
+      <c r="E9" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="F9" s="5">
+        <v>7</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="J9" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$17,B9+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$21,B9+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$25,B9+2))="n","Z, ","")</f>
+        <v xml:space="preserve">Z, </v>
+      </c>
+      <c r="K9" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$18,B9+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$22,B9+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$26,B9+2))="n","Z, ","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="5">
+        <v>8</v>
+      </c>
+      <c r="C10" s="31" t="str">
+        <f ca="1">IF(J10="","",SUBSTITUTE(J10,", ","",(LEN(J10)-LEN(SUBSTITUTE(J10,", ","")))/2))</f>
+        <v>X, Y, Z</v>
+      </c>
+      <c r="D10" s="5">
+        <v>8</v>
+      </c>
+      <c r="E10" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="F10" s="5">
+        <v>8</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="J10" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$17,B10+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$21,B10+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$25,B10+2))="n","Z, ","")</f>
+        <v xml:space="preserve">X, Y, Z, </v>
+      </c>
+      <c r="K10" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$18,B10+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$22,B10+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$26,B10+2))="n","Z, ","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="5">
+        <v>9</v>
+      </c>
+      <c r="C11" s="31" t="str">
+        <f ca="1">IF(J11="","",SUBSTITUTE(J11,", ","",(LEN(J11)-LEN(SUBSTITUTE(J11,", ","")))/2))</f>
+        <v/>
+      </c>
+      <c r="D11" s="5">
+        <v>9</v>
+      </c>
+      <c r="E11" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>X, Y, Z</v>
+      </c>
+      <c r="F11" s="5">
+        <v>9</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="J11" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$17,B11+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$21,B11+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$25,B11+2))="n","Z, ","")</f>
+        <v/>
+      </c>
+      <c r="K11" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$18,B11+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$22,B11+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$26,B11+2))="n","Z, ","")</f>
+        <v xml:space="preserve">X, Y, Z, </v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="5">
+        <v>10</v>
+      </c>
+      <c r="C12" s="31" t="str">
+        <f ca="1">IF(J12="","",SUBSTITUTE(J12,", ","",(LEN(J12)-LEN(SUBSTITUTE(J12,", ","")))/2))</f>
+        <v>X</v>
+      </c>
+      <c r="D12" s="5">
+        <v>10</v>
+      </c>
+      <c r="E12" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Z</v>
+      </c>
+      <c r="F12" s="5">
+        <v>10</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="J12" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$17,B12+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$21,B12+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$25,B12+2))="n","Z, ","")</f>
+        <v xml:space="preserve">X, </v>
+      </c>
+      <c r="K12" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$18,B12+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$22,B12+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$26,B12+2))="n","Z, ","")</f>
+        <v xml:space="preserve">Z, </v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="5">
+        <v>11</v>
+      </c>
+      <c r="C13" s="31" t="str">
+        <f ca="1">IF(J13="","",SUBSTITUTE(J13,", ","",(LEN(J13)-LEN(SUBSTITUTE(J13,", ","")))/2))</f>
+        <v>X</v>
+      </c>
+      <c r="D13" s="5">
+        <v>11</v>
+      </c>
+      <c r="E13" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>X, Y, Z</v>
+      </c>
+      <c r="F13" s="5">
+        <v>11</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="J13" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$17,B13+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$21,B13+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$25,B13+2))="n","Z, ","")</f>
+        <v xml:space="preserve">X, </v>
+      </c>
+      <c r="K13" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$18,B13+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$22,B13+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$26,B13+2))="n","Z, ","")</f>
+        <v xml:space="preserve">X, Y, Z, </v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="5">
+        <v>12</v>
+      </c>
+      <c r="C14" s="31" t="str">
+        <f ca="1">IF(J14="","",SUBSTITUTE(J14,", ","",(LEN(J14)-LEN(SUBSTITUTE(J14,", ","")))/2))</f>
+        <v>X, Y, Z</v>
+      </c>
+      <c r="D14" s="5">
+        <v>12</v>
+      </c>
+      <c r="E14" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="F14" s="5">
+        <v>12</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="J14" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$17,B14+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$21,B14+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$25,B14+2))="n","Z, ","")</f>
+        <v xml:space="preserve">X, Y, Z, </v>
+      </c>
+      <c r="K14" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$18,B14+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$22,B14+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$26,B14+2))="n","Z, ","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="5">
+        <v>13</v>
+      </c>
+      <c r="C15" s="31" t="str">
+        <f ca="1">IF(J15="","",SUBSTITUTE(J15,", ","",(LEN(J15)-LEN(SUBSTITUTE(J15,", ","")))/2))</f>
+        <v/>
+      </c>
+      <c r="D15" s="5">
+        <v>13</v>
+      </c>
+      <c r="E15" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="F15" s="5">
+        <v>13</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="J15" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$17,B15+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$21,B15+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$25,B15+2))="n","Z, ","")</f>
+        <v/>
+      </c>
+      <c r="K15" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$18,B15+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$22,B15+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$26,B15+2))="n","Z, ","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="5">
+        <v>14</v>
+      </c>
+      <c r="C16" s="31" t="str">
+        <f ca="1">IF(J16="","",SUBSTITUTE(J16,", ","",(LEN(J16)-LEN(SUBSTITUTE(J16,", ","")))/2))</f>
+        <v/>
+      </c>
+      <c r="D16" s="5">
+        <v>14</v>
+      </c>
+      <c r="E16" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="F16" s="5">
+        <v>14</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="J16" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$17,B16+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$21,B16+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$25,B16+2))="n","Z, ","")</f>
+        <v/>
+      </c>
+      <c r="K16" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$18,B16+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$22,B16+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$26,B16+2))="n","Z, ","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="5">
+        <v>15</v>
+      </c>
+      <c r="C17" s="31" t="str">
+        <f ca="1">IF(J17="","",SUBSTITUTE(J17,", ","",(LEN(J17)-LEN(SUBSTITUTE(J17,", ","")))/2))</f>
+        <v>X, Y, Z</v>
+      </c>
+      <c r="D17" s="5">
+        <v>15</v>
+      </c>
+      <c r="E17" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Y</v>
+      </c>
+      <c r="F17" s="5">
+        <v>15</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="J17" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$17,B17+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$21,B17+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$25,B17+2))="n","Z, ","")</f>
+        <v xml:space="preserve">X, Y, Z, </v>
+      </c>
+      <c r="K17" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$18,B17+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$22,B17+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$26,B17+2))="n","Z, ","")</f>
+        <v xml:space="preserve">Y, </v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="5">
+        <v>16</v>
+      </c>
+      <c r="C18" s="31" t="str">
+        <f ca="1">IF(J18="","",SUBSTITUTE(J18,", ","",(LEN(J18)-LEN(SUBSTITUTE(J18,", ","")))/2))</f>
+        <v/>
+      </c>
+      <c r="D18" s="5">
+        <v>16</v>
+      </c>
+      <c r="E18" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>X, Y, Z</v>
+      </c>
+      <c r="F18" s="5">
+        <v>16</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="J18" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$17,B18+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$21,B18+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$25,B18+2))="n","Z, ","")</f>
+        <v/>
+      </c>
+      <c r="K18" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$18,B18+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$22,B18+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$26,B18+2))="n","Z, ","")</f>
+        <v xml:space="preserve">X, Y, Z, </v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="5">
+        <v>17</v>
+      </c>
+      <c r="C19" s="31" t="str">
+        <f ca="1">IF(J19="","",SUBSTITUTE(J19,", ","",(LEN(J19)-LEN(SUBSTITUTE(J19,", ","")))/2))</f>
+        <v/>
+      </c>
+      <c r="D19" s="5">
+        <v>17</v>
+      </c>
+      <c r="E19" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Y</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="J19" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$17,B19+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$21,B19+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$25,B19+2))="n","Z, ","")</f>
+        <v/>
+      </c>
+      <c r="K19" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$18,B19+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$22,B19+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$26,B19+2))="n","Z, ","")</f>
+        <v xml:space="preserve">Y, </v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="5">
+        <v>18</v>
+      </c>
+      <c r="C20" s="31" t="str">
+        <f ca="1">IF(J20="","",SUBSTITUTE(J20,", ","",(LEN(J20)-LEN(SUBSTITUTE(J20,", ","")))/2))</f>
+        <v>X, Y, Z</v>
+      </c>
+      <c r="D20" s="5">
+        <v>18</v>
+      </c>
+      <c r="E20" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="J20" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$17,B20+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$21,B20+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$25,B20+2))="n","Z, ","")</f>
+        <v xml:space="preserve">X, Y, Z, </v>
+      </c>
+      <c r="K20" s="32" t="str">
+        <f ca="1">IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$18,B20+2))="n","X, ","")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$22,B20+2))="n","Y, ", "")&amp;IF(INDIRECT("Sheet1!"&amp;ADDRESS(Sheet1!$A$26,B20+2))="n","Z, ","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>